<commit_message>
miguelito, vamos por amortig y frec natural
</commit_message>
<xml_diff>
--- a/Matlab - Simulink/Tabla_Polos_Temperatura.xlsx
+++ b/Matlab - Simulink/Tabla_Polos_Temperatura.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B584C-FF17-455E-BCD2-81343A9EFB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -25,7 +25,238 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>Rs_Ohm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ceros</t>
+  </si>
+  <si>
+    <t>wn_rad_s</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
   <si>
     <t>Rs_Ohm</t>
   </si>
@@ -66,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,12 +305,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,224 +629,226 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="3" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="true"/>
+    <col min="2" max="2" width="3.28515625" customWidth="true"/>
+    <col min="3" max="3" width="12.42578125" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.42578125" customWidth="true"/>
+    <col min="5" max="5" width="12.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1.0995600000000001</v>
+      </c>
+      <c r="B2" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="C2" s="0">
+        <v>-95.291585674344304</v>
+      </c>
+      <c r="D2" s="0">
+        <v>-95.291585674344304</v>
+      </c>
+      <c r="E2" s="0">
+        <v>-189.5793103448276</v>
+      </c>
+      <c r="F2" s="0">
+        <v>174.0907631319642</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0.54736726957829129</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>1.0995600000000001</v>
-      </c>
-      <c r="B2">
+    <row r="3">
+      <c r="A3" s="0">
+        <v>1.13934</v>
+      </c>
+      <c r="B3" s="0">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>-95.344235726994356</v>
-      </c>
-      <c r="D2">
-        <v>-95.344235726994356</v>
-      </c>
-      <c r="E2">
-        <v>-189.5793103448276</v>
-      </c>
-      <c r="F2">
-        <v>174.14808792866981</v>
-      </c>
-      <c r="G2">
-        <v>0.54748942041813797</v>
+      <c r="C3" s="0">
+        <v>-98.720896019171889</v>
+      </c>
+      <c r="D3" s="0">
+        <v>-98.720896019171889</v>
+      </c>
+      <c r="E3" s="0">
+        <v>-196.43793103448277</v>
+      </c>
+      <c r="F3" s="0">
+        <v>174.11053646956663</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.5670012741384417</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>1.13934</v>
-      </c>
-      <c r="B3">
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1.1791199999999999</v>
+      </c>
+      <c r="B4" s="0">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>-98.77354607182194</v>
-      </c>
-      <c r="D3">
-        <v>-98.77354607182194</v>
-      </c>
-      <c r="E3">
-        <v>-196.43793103448277</v>
-      </c>
-      <c r="F3">
-        <v>174.16992807182058</v>
-      </c>
-      <c r="G3">
-        <v>0.56711021911366788</v>
+      <c r="C4" s="0">
+        <v>-102.15020636399947</v>
+      </c>
+      <c r="D4" s="0">
+        <v>-102.15020636399947</v>
+      </c>
+      <c r="E4" s="0">
+        <v>-203.29655172413794</v>
+      </c>
+      <c r="F4" s="0">
+        <v>174.13030756181104</v>
+      </c>
+      <c r="G4" s="0">
+        <v>0.58663082719094839</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>1.1791199999999999</v>
-      </c>
-      <c r="B4">
+    <row r="5">
+      <c r="A5" s="0">
+        <v>1.2189000000000001</v>
+      </c>
+      <c r="B5" s="0">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>-102.20285641664952</v>
-      </c>
-      <c r="D4">
-        <v>-102.20285641664952</v>
-      </c>
-      <c r="E4">
-        <v>-203.29655172413794</v>
-      </c>
-      <c r="F4">
-        <v>174.19176547665683</v>
-      </c>
-      <c r="G4">
-        <v>0.58672610692579252</v>
+      <c r="C5" s="0">
+        <v>-105.57951670882706</v>
+      </c>
+      <c r="D5" s="0">
+        <v>-105.57951670882706</v>
+      </c>
+      <c r="E5" s="0">
+        <v>-210.15517241379314</v>
+      </c>
+      <c r="F5" s="0">
+        <v>174.1500764094622</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.60625593100854103</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>1.2189000000000001</v>
-      </c>
-      <c r="B5">
+    <row r="6">
+      <c r="A6" s="0">
+        <v>1.25868</v>
+      </c>
+      <c r="B6" s="0">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>-105.63216676147711</v>
-      </c>
-      <c r="D5">
-        <v>-105.63216676147711</v>
-      </c>
-      <c r="E5">
-        <v>-210.15517241379314</v>
-      </c>
-      <c r="F5">
-        <v>174.21360014420821</v>
-      </c>
-      <c r="G5">
-        <v>0.60633708662261909</v>
+      <c r="C6" s="0">
+        <v>-109.00882705365464</v>
+      </c>
+      <c r="D6" s="0">
+        <v>-109.00882705365464</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-217.01379310344831</v>
+      </c>
+      <c r="F6" s="0">
+        <v>174.16984301328441</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0.62587658786222966</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>1.25868</v>
-      </c>
-      <c r="B6">
+    <row r="7">
+      <c r="A7" s="0">
+        <v>1.2984599999999999</v>
+      </c>
+      <c r="B7" s="0">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>-109.06147710630469</v>
-      </c>
-      <c r="D6">
-        <v>-109.06147710630469</v>
-      </c>
-      <c r="E6">
-        <v>-217.01379310344831</v>
-      </c>
-      <c r="F6">
-        <v>174.23543207550384</v>
-      </c>
-      <c r="G6">
-        <v>0.62594316096994318</v>
+      <c r="C7" s="0">
+        <v>-112.43813739848223</v>
+      </c>
+      <c r="D7" s="0">
+        <v>-112.43813739848223</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-223.87241379310345</v>
+      </c>
+      <c r="F7" s="0">
+        <v>174.1896073740416</v>
+      </c>
+      <c r="G7" s="0">
+        <v>0.64549280002130704</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>1.2984599999999999</v>
-      </c>
-      <c r="B7">
+    <row r="8">
+      <c r="A8" s="0">
+        <v>1.3382400000000001</v>
+      </c>
+      <c r="B8" s="0">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>-112.49078745113228</v>
-      </c>
-      <c r="D7">
-        <v>-112.49078745113228</v>
-      </c>
-      <c r="E7">
-        <v>-223.87241379310345</v>
-      </c>
-      <c r="F7">
-        <v>174.25726127157219</v>
-      </c>
-      <c r="G7">
-        <v>0.64554433273125067</v>
+      <c r="C8" s="0">
+        <v>-115.86744774330982</v>
+      </c>
+      <c r="D8" s="0">
+        <v>-115.86744774330982</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-230.73103448275864</v>
+      </c>
+      <c r="F8" s="0">
+        <v>174.2093694924971</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0.66510456975335097</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>1.3382400000000001</v>
-      </c>
-      <c r="B8">
+    <row r="9">
+      <c r="A9" s="0">
+        <v>1.37802</v>
+      </c>
+      <c r="B9" s="0">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>-115.92009779595986</v>
-      </c>
-      <c r="D8">
-        <v>-115.92009779595986</v>
-      </c>
-      <c r="E8">
-        <v>-230.73103448275864</v>
-      </c>
-      <c r="F8">
-        <v>174.279087733441</v>
-      </c>
-      <c r="G8">
-        <v>0.66514060466772162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>1.37802</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>-119.34940814078745</v>
-      </c>
-      <c r="D9">
-        <v>-119.34940814078745</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="0">
+        <v>-119.29675808813739</v>
+      </c>
+      <c r="D9" s="0">
+        <v>-119.29675808813739</v>
+      </c>
+      <c r="E9" s="0">
         <v>-237.58965517241381</v>
       </c>
-      <c r="F9">
-        <v>174.30091146213746</v>
-      </c>
-      <c r="G9">
-        <v>0.68473197953823173</v>
+      <c r="F9" s="0">
+        <v>174.22912936941401</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.68471189932422394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>